<commit_message>
Listado de Acividades Modificado
</commit_message>
<xml_diff>
--- a/Listada de Actividades.xlsx
+++ b/Listada de Actividades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>locutor</t>
+  </si>
+  <si>
+    <t>2 dias</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,6 +252,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,7 +539,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,10 +593,14 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="F2" s="17">
+        <v>42408</v>
+      </c>
+      <c r="G2" s="17">
+        <v>42410</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
@@ -609,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -968,8 +978,12 @@
       <c r="E19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="17">
+        <v>42510</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H19" s="2" t="s">
         <v>35</v>
       </c>

</xml_diff>